<commit_message>
updating project file list
</commit_message>
<xml_diff>
--- a/project management/gantt chart.xlsx
+++ b/project management/gantt chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="1160" windowWidth="35000" windowHeight="27120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21720" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="147">
   <si>
     <t>TAU data</t>
   </si>
@@ -111,9 +111,6 @@
     <t>syn3157182</t>
   </si>
   <si>
-    <t>JNPL3 &amp; rTG data</t>
-  </si>
-  <si>
     <t>MayoEGWAS_UFL-Mayo-ISB_IlluminaWholeGenomeDASL_Cerebellum</t>
   </si>
   <si>
@@ -297,9 +294,6 @@
     <t>syn3219036</t>
   </si>
   <si>
-    <t>What is the difference between the 2 synapse objects?</t>
-  </si>
-  <si>
     <t>syn3157238</t>
   </si>
   <si>
@@ -370,13 +364,109 @@
   </si>
   <si>
     <t>syn2430570</t>
+  </si>
+  <si>
+    <t>syn3207163</t>
+  </si>
+  <si>
+    <t>syn3207165</t>
+  </si>
+  <si>
+    <t>syn3207167</t>
+  </si>
+  <si>
+    <t>syn3207169</t>
+  </si>
+  <si>
+    <t>syn3207173</t>
+  </si>
+  <si>
+    <t>syn3207175</t>
+  </si>
+  <si>
+    <t>syn3207177</t>
+  </si>
+  <si>
+    <t>syn3207179</t>
+  </si>
+  <si>
+    <t>syn3207181</t>
+  </si>
+  <si>
+    <t>syn3207183</t>
+  </si>
+  <si>
+    <t>syn3207185</t>
+  </si>
+  <si>
+    <t>syn3207187</t>
+  </si>
+  <si>
+    <t>syn3218794</t>
+  </si>
+  <si>
+    <t>syn3218985</t>
+  </si>
+  <si>
+    <t>syn3218987</t>
+  </si>
+  <si>
+    <t>syn3218989</t>
+  </si>
+  <si>
+    <t>syn3218991</t>
+  </si>
+  <si>
+    <t>syn3218993</t>
+  </si>
+  <si>
+    <t>syn3218995</t>
+  </si>
+  <si>
+    <t>syn3218997</t>
+  </si>
+  <si>
+    <t>syn3218999</t>
+  </si>
+  <si>
+    <t>syn3218797</t>
+  </si>
+  <si>
+    <t>syn3219001</t>
+  </si>
+  <si>
+    <t>syn3219003</t>
+  </si>
+  <si>
+    <t>syn3219005</t>
+  </si>
+  <si>
+    <t>syn3219007</t>
+  </si>
+  <si>
+    <t>syn3219018</t>
+  </si>
+  <si>
+    <t>syn3219020</t>
+  </si>
+  <si>
+    <t>syn3219022</t>
+  </si>
+  <si>
+    <t>JNPL3 &amp; rTG data - mouse-tau-rnaseq directory</t>
+  </si>
+  <si>
+    <t>mouse-app-rnaseq directory</t>
+  </si>
+  <si>
+    <t>Tau and APP mouse model study - TAUAPPms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -413,6 +503,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -441,7 +539,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -466,6 +564,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -484,7 +586,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="24">
+  <cellStyles count="28">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -507,12 +609,2221 @@
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="13906500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="14097000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1027" name="AutoShape 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="14097000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1028" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="14287500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1029" name="AutoShape 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="14287500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1030" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="8191500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1031" name="AutoShape 7"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="8382000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1032" name="AutoShape 8"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="8382000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1033" name="AutoShape 9"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="8191500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1034" name="AutoShape 10"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="8572500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1035" name="AutoShape 11"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="8763000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1036" name="AutoShape 12"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="8763000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1037" name="AutoShape 13"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="8953500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1038" name="AutoShape 14"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="8953500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1039" name="AutoShape 15"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="9144000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1040" name="AutoShape 16"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="9144000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1041" name="AutoShape 17"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="9334500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1042" name="AutoShape 18"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="9334500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1043" name="AutoShape 19"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="9525000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1044" name="AutoShape 20"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="9525000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1045" name="AutoShape 21"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="9715500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1046" name="AutoShape 22"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="9715500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1047" name="AutoShape 23"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="9906000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1048" name="AutoShape 24"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="9906000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1049" name="AutoShape 25"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="10096500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1050" name="AutoShape 26"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="10096500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1051" name="AutoShape 27"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="10287000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1052" name="AutoShape 28"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="10287000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1053" name="AutoShape 29"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="5905500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1054" name="AutoShape 30"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="5905500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1055" name="AutoShape 31"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="6096000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1056" name="AutoShape 32"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="6096000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1057" name="AutoShape 33"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="6286500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1058" name="AutoShape 34"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6502400" y="5334000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1059" name="AutoShape 35"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6502400" y="6477000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1060" name="AutoShape 36"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="6477000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1061" name="AutoShape 37"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6502400" y="6667500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1062" name="AutoShape 38"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="6667500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1063" name="AutoShape 39"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="7239000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1064" name="AutoShape 40"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="7239000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1065" name="AutoShape 41"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="7429500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1066" name="AutoShape 42"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="7429500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1067" name="AutoShape 43"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="7620000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1068" name="AutoShape 44"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="7620000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -836,14 +3147,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -870,13 +3181,10 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
       <c r="B3" t="s">
         <v>29</v>
       </c>
@@ -886,47 +3194,44 @@
       <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
-        <v>92</v>
+      <c r="H3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>30</v>
+        <v>144</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H6" t="s">
         <v>22</v>
@@ -934,10 +3239,10 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H7" t="s">
         <v>23</v>
@@ -945,24 +3250,24 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>24</v>
       </c>
       <c r="I8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H9" t="s">
         <v>25</v>
@@ -970,10 +3275,10 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
@@ -981,22 +3286,25 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>27</v>
       </c>
       <c r="I11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="G13" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="H13" s="4" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1">
       <c r="H14" s="4" t="s">
@@ -1005,22 +3313,22 @@
     </row>
     <row r="15" spans="1:9" s="4" customFormat="1">
       <c r="H15" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1">
       <c r="H16" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1">
       <c r="H17" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="4" customFormat="1">
       <c r="H18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1036,50 +3344,50 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E21" s="2"/>
       <c r="H21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E22" s="2"/>
       <c r="H22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E23" s="2"/>
       <c r="H23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E24" s="2"/>
       <c r="H24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1098,110 +3406,110 @@
     </row>
     <row r="27" spans="1:9" ht="45">
       <c r="B27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E27" s="2"/>
       <c r="G27" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E28" s="2"/>
       <c r="H28" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I28" s="7"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E29" s="2"/>
       <c r="H29" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E30" s="2"/>
       <c r="H30" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E31" s="2"/>
       <c r="H31" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:9" ht="45">
       <c r="B32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E32" s="2"/>
       <c r="G32" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E33" s="2"/>
       <c r="H33" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I33" s="7"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E34" s="2"/>
       <c r="H34" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E35" s="2"/>
       <c r="H35" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I35" s="7"/>
     </row>
@@ -1222,92 +3530,128 @@
       </c>
     </row>
     <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>115</v>
+      </c>
       <c r="E38" s="2"/>
       <c r="H38" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>116</v>
+      </c>
       <c r="E39" s="2"/>
       <c r="H39" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I39" s="7"/>
     </row>
     <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
       <c r="E40" s="2"/>
       <c r="H40" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I40" s="7"/>
     </row>
     <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>118</v>
+      </c>
       <c r="E41" s="2"/>
       <c r="H41" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>119</v>
+      </c>
       <c r="E42" s="2"/>
       <c r="H42" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>120</v>
+      </c>
       <c r="E43" s="2"/>
       <c r="H43" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I43" s="7"/>
     </row>
     <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>121</v>
+      </c>
       <c r="E44" s="2"/>
       <c r="H44" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I44" s="7"/>
     </row>
     <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>122</v>
+      </c>
       <c r="E45" s="2"/>
       <c r="H45" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>123</v>
+      </c>
       <c r="E46" s="2"/>
       <c r="H46" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>124</v>
+      </c>
       <c r="E47" s="2"/>
       <c r="H47" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>125</v>
+      </c>
       <c r="E48" s="2"/>
       <c r="H48" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="2:9">
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>126</v>
+      </c>
       <c r="E49" s="2"/>
       <c r="H49" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I49" s="7"/>
     </row>
-    <row r="50" spans="2:9">
+    <row r="50" spans="1:9">
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="1:9">
       <c r="B51" t="s">
         <v>17</v>
       </c>
@@ -1321,88 +3665,130 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>127</v>
+      </c>
       <c r="E52" s="1"/>
       <c r="H52" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>128</v>
+      </c>
       <c r="E53" s="1"/>
       <c r="H53" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>132</v>
+      </c>
       <c r="E54" s="1"/>
       <c r="H54" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>133</v>
+      </c>
       <c r="E55" s="1"/>
       <c r="H55" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>129</v>
+      </c>
       <c r="E56" s="1"/>
       <c r="H56" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>134</v>
+      </c>
       <c r="E57" s="1"/>
       <c r="H57" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>135</v>
+      </c>
       <c r="E58" s="1"/>
       <c r="H58" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="59" spans="2:9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>136</v>
+      </c>
       <c r="E59" s="1"/>
       <c r="H59" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>130</v>
+      </c>
       <c r="E60" s="1"/>
       <c r="H60" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="61" spans="2:9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>137</v>
+      </c>
       <c r="E61" s="1"/>
       <c r="H61" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="62" spans="2:9">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>138</v>
+      </c>
       <c r="E62" s="1"/>
       <c r="H62" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="63" spans="2:9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>131</v>
+      </c>
       <c r="E63" s="1"/>
       <c r="H63" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="64" spans="2:9">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>139</v>
+      </c>
       <c r="E64" s="1"/>
       <c r="H64" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>140</v>
+      </c>
       <c r="E65" s="1"/>
       <c r="H65" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -1424,22 +3810,31 @@
       </c>
     </row>
     <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>143</v>
+      </c>
       <c r="E68" s="1"/>
       <c r="H68" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>141</v>
+      </c>
       <c r="E69" s="1"/>
       <c r="H69" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I69" s="7"/>
     </row>
     <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>142</v>
+      </c>
       <c r="E70" s="1"/>
       <c r="H70" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I70" s="7"/>
     </row>
@@ -1465,25 +3860,25 @@
     <row r="74" spans="1:9" s="4" customFormat="1">
       <c r="E74" s="6"/>
       <c r="H74" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="4" customFormat="1">
       <c r="E75" s="6"/>
       <c r="H75" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="4" customFormat="1">
       <c r="E76" s="6"/>
       <c r="H76" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="4" customFormat="1">
       <c r="E77" s="6"/>
       <c r="H77" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -1508,7 +3903,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
working on MBB_TCX covariates
</commit_message>
<xml_diff>
--- a/project management/gantt chart.xlsx
+++ b/project management/gantt chart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="190">
   <si>
     <t>TAU data</t>
   </si>
@@ -54,9 +54,6 @@
     <t>IL10 Nanostring expression</t>
   </si>
   <si>
-    <t>MayoBB RNA-seq</t>
-  </si>
-  <si>
     <t>MayoLOADGWAS Exome sequencing</t>
   </si>
   <si>
@@ -508,6 +505,90 @@
   </si>
   <si>
     <t>syn3483625</t>
+  </si>
+  <si>
+    <t>syn3505856</t>
+  </si>
+  <si>
+    <t>syn3505860</t>
+  </si>
+  <si>
+    <t>syn2910240</t>
+  </si>
+  <si>
+    <t>U Florida - Mayo Clinic - ISB folder</t>
+  </si>
+  <si>
+    <t>syn2397885</t>
+  </si>
+  <si>
+    <t>I think this is my public root directory. (not sure of working id)</t>
+  </si>
+  <si>
+    <t>I think this release is the TCX (temporal cotex) samples, n = 399?</t>
+  </si>
+  <si>
+    <t>(I think this should be the CER (cerebellum) samples, n = 374?</t>
+  </si>
+  <si>
+    <t>Working Synapse ID - study info</t>
+  </si>
+  <si>
+    <t>syn3163039</t>
+  </si>
+  <si>
+    <t>Mayo RNA-seq</t>
+  </si>
+  <si>
+    <t>syn2875332</t>
+  </si>
+  <si>
+    <t>mayo-tcx-rna-seq</t>
+  </si>
+  <si>
+    <t>mayo-cer-rna-seq</t>
+  </si>
+  <si>
+    <t>parent of pilot studies, cer, and tcx samples</t>
+  </si>
+  <si>
+    <t>syn3191070</t>
+  </si>
+  <si>
+    <t>syn3191083</t>
+  </si>
+  <si>
+    <t>syn3160436</t>
+  </si>
+  <si>
+    <t>syn3160437</t>
+  </si>
+  <si>
+    <t>syn3160443</t>
+  </si>
+  <si>
+    <t>syn3191085</t>
+  </si>
+  <si>
+    <t>syn3160444</t>
+  </si>
+  <si>
+    <t>syn3191122</t>
+  </si>
+  <si>
+    <t>"Mayo BB samples"</t>
+  </si>
+  <si>
+    <t>"mouse data"</t>
+  </si>
+  <si>
+    <t>syn3509411</t>
+  </si>
+  <si>
+    <t>syn2910255</t>
+  </si>
+  <si>
+    <t>syn2924460 (or syn2924461 ?)</t>
   </si>
 </sst>
 </file>
@@ -593,7 +674,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -640,8 +721,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -658,8 +748,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="46">
+  <cellStyles count="55">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -693,6 +786,13 @@
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
@@ -704,6 +804,8 @@
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -718,13 +820,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -768,13 +870,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -818,13 +920,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -868,13 +970,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -918,13 +1020,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -937,56 +1039,6 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="15303500" y="14287500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1030" name="AutoShape 6"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="8191500"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1029,6 +1081,56 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
+        <xdr:cNvPr id="1030" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="8191500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
         <xdr:cNvPr id="1031" name="AutoShape 7"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -1068,67 +1170,67 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1032" name="AutoShape 8"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="8382000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1032" name="AutoShape 8"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15303500" y="8382000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
         <xdr:cNvPr id="1033" name="AutoShape 9"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -1168,125 +1270,25 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1034" name="AutoShape 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15303500" y="8572500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1035" name="AutoShape 11"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="8763000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1036" name="AutoShape 12"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15303500" y="8763000"/>
+        <xdr:cNvPr id="1034" name="AutoShape 10"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="8572500"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1329,14 +1331,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1037" name="AutoShape 13"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="8953500"/>
+        <xdr:cNvPr id="1035" name="AutoShape 11"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="8763000"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1379,14 +1381,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1038" name="AutoShape 14"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15303500" y="8953500"/>
+        <xdr:cNvPr id="1036" name="AutoShape 12"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="8763000"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1429,14 +1431,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1039" name="AutoShape 15"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="9144000"/>
+        <xdr:cNvPr id="1037" name="AutoShape 13"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="8953500"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1479,14 +1481,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1040" name="AutoShape 16"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15303500" y="9144000"/>
+        <xdr:cNvPr id="1038" name="AutoShape 14"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="8953500"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1529,14 +1531,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1041" name="AutoShape 17"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="9334500"/>
+        <xdr:cNvPr id="1039" name="AutoShape 15"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="9144000"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1579,14 +1581,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1042" name="AutoShape 18"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15303500" y="9334500"/>
+        <xdr:cNvPr id="1040" name="AutoShape 16"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="9144000"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1629,14 +1631,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1043" name="AutoShape 19"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="9525000"/>
+        <xdr:cNvPr id="1041" name="AutoShape 17"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="9334500"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1679,14 +1681,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1044" name="AutoShape 20"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15303500" y="9525000"/>
+        <xdr:cNvPr id="1042" name="AutoShape 18"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="9334500"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1729,14 +1731,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1045" name="AutoShape 21"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="9715500"/>
+        <xdr:cNvPr id="1043" name="AutoShape 19"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="9525000"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1779,14 +1781,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1046" name="AutoShape 22"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15303500" y="9715500"/>
+        <xdr:cNvPr id="1044" name="AutoShape 20"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="9525000"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1829,14 +1831,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1047" name="AutoShape 23"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="9906000"/>
+        <xdr:cNvPr id="1045" name="AutoShape 21"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="9715500"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1879,14 +1881,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1048" name="AutoShape 24"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15303500" y="9906000"/>
+        <xdr:cNvPr id="1046" name="AutoShape 22"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="9715500"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1929,14 +1931,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1049" name="AutoShape 25"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="10096500"/>
+        <xdr:cNvPr id="1047" name="AutoShape 23"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="9906000"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1979,14 +1981,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1050" name="AutoShape 26"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15303500" y="10096500"/>
+        <xdr:cNvPr id="1048" name="AutoShape 24"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="9906000"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2029,14 +2031,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1051" name="AutoShape 27"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="10287000"/>
+        <xdr:cNvPr id="1049" name="AutoShape 25"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="10096500"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2079,6 +2081,106 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
+        <xdr:cNvPr id="1050" name="AutoShape 26"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="10096500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1051" name="AutoShape 27"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="10287000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
         <xdr:cNvPr id="1052" name="AutoShape 28"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -2087,106 +2189,6 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="15303500" y="10287000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1053" name="AutoShape 29"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="5905500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1054" name="AutoShape 30"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15303500" y="5905500"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2229,64 +2231,64 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1055" name="AutoShape 31"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="6096000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
+        <xdr:cNvPr id="1053" name="AutoShape 29"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="5905500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1056" name="AutoShape 32"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="6096000"/>
+        <xdr:cNvPr id="1054" name="AutoShape 30"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="5905500"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2329,106 +2331,206 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1057" name="AutoShape 33"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="6286500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1058" name="AutoShape 34"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6502400" y="5334000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+        <xdr:cNvPr id="1055" name="AutoShape 31"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="6096000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1056" name="AutoShape 32"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="6096000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
+        <xdr:cNvPr id="1057" name="AutoShape 33"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="6286500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1058" name="AutoShape 34"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6502400" y="5334000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
         <xdr:cNvPr id="1059" name="AutoShape 35"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -2468,13 +2570,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2518,13 +2620,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2568,13 +2670,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2587,106 +2689,6 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="15303500" y="6667500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1063" name="AutoShape 39"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="7239000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1064" name="AutoShape 40"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15303500" y="7239000"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2729,14 +2731,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1065" name="AutoShape 41"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7327900" y="7429500"/>
+        <xdr:cNvPr id="1063" name="AutoShape 39"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="7239000"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2779,14 +2781,14 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1066" name="AutoShape 42"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15303500" y="7429500"/>
+        <xdr:cNvPr id="1064" name="AutoShape 40"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="7239000"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2829,6 +2831,106 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
+        <xdr:cNvPr id="1065" name="AutoShape 41"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7327900" y="7429500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1066" name="AutoShape 42"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15303500" y="7429500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
         <xdr:cNvPr id="1067" name="AutoShape 43"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -2868,13 +2970,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3239,57 +3341,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="104.6640625" customWidth="1"/>
     <col min="9" max="9" width="68.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="45">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>170</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E3" s="2">
-        <v>42050</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>144</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3299,739 +3399,831 @@
       <c r="D4" t="s">
         <v>145</v>
       </c>
+      <c r="E4" s="2">
+        <v>42050</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
       <c r="G4" t="s">
+        <v>186</v>
+      </c>
+      <c r="H4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G5" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" t="s">
-        <v>148</v>
-      </c>
-      <c r="H5" t="s">
-        <v>149</v>
+      <c r="H5" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="I5" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="I6" t="s">
-        <v>81</v>
+        <v>147</v>
+      </c>
+      <c r="H6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
-      </c>
-      <c r="H7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>158</v>
+      </c>
+      <c r="I7" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" t="s">
-        <v>80</v>
+        <v>102</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
         <v>104</v>
       </c>
-      <c r="H10" t="s">
-        <v>23</v>
+      <c r="H10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="8" customFormat="1">
-      <c r="D14" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G14" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="8" customFormat="1">
+      <c r="D15" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="8" customFormat="1">
-      <c r="C15" s="8" t="s">
-        <v>152</v>
-      </c>
       <c r="H15" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="8" customFormat="1">
+      <c r="C16" s="8" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" s="4" customFormat="1">
-      <c r="C16" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>160</v>
+      <c r="H16" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1">
       <c r="C17" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="4" customFormat="1">
-      <c r="H18" s="9" t="s">
-        <v>154</v>
+      <c r="C18" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="4" customFormat="1">
       <c r="C19" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="4" customFormat="1">
+      <c r="C20" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="4" customFormat="1">
+      <c r="C21" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="4" customFormat="1">
-      <c r="H20" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="2">
+    <row r="23" spans="1:9">
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="2">
         <v>42050</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" t="s">
-        <v>107</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="H23" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E24" s="2"/>
       <c r="H24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E25" s="2"/>
       <c r="H25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E26" s="2"/>
       <c r="H26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
       <c r="E27" s="2"/>
+      <c r="H27" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="B28" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="2">
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="2">
         <v>42050</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="45">
-      <c r="B29" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="G29" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" t="s">
-        <v>109</v>
+    <row r="30" spans="1:9" ht="30">
+      <c r="B30" t="s">
+        <v>88</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="H30" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="I30" s="7"/>
+      <c r="G30" s="5" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E31" s="2"/>
       <c r="H31" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E32" s="2"/>
       <c r="H32" s="5" t="s">
-        <v>68</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E33" s="2"/>
       <c r="H33" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="H34" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" ht="30">
+      <c r="B35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="G35" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="I33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" ht="45">
-      <c r="B34" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" s="2"/>
-      <c r="G34" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I34" s="7"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" t="s">
-        <v>96</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="H35" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="I35" s="7"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E36" s="2"/>
       <c r="H36" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I36" s="7"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E37" s="2"/>
       <c r="H37" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I37" s="7"/>
     </row>
     <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" t="s">
+        <v>99</v>
+      </c>
       <c r="E38" s="2"/>
-      <c r="H38" s="5"/>
+      <c r="H38" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="I38" s="7"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="B39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="2">
+      <c r="E39" s="2"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="2">
         <v>42050</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" t="s">
-        <v>113</v>
-      </c>
-      <c r="E40" s="2"/>
-      <c r="H40" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E41" s="2"/>
       <c r="H41" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I41" s="7"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E42" s="2"/>
       <c r="H42" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E43" s="2"/>
       <c r="H43" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I43" s="7"/>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E44" s="2"/>
       <c r="H44" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I44" s="7"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E45" s="2"/>
       <c r="H45" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E46" s="2"/>
       <c r="H46" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E47" s="2"/>
       <c r="H47" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E48" s="2"/>
       <c r="H48" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I48" s="7"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E49" s="2"/>
       <c r="H49" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I49" s="7"/>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E50" s="2"/>
       <c r="H50" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I50" s="7"/>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E51" s="2"/>
       <c r="H51" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I51" s="7"/>
     </row>
     <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>123</v>
+      </c>
       <c r="E52" s="2"/>
+      <c r="H52" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I52" s="7"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="B53" t="s">
-        <v>17</v>
-      </c>
-      <c r="E53" s="1">
-        <v>42036</v>
-      </c>
-      <c r="F53" t="s">
-        <v>8</v>
-      </c>
-      <c r="G53" t="s">
-        <v>9</v>
-      </c>
+      <c r="E53" s="1"/>
+      <c r="H53" s="5"/>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>125</v>
-      </c>
-      <c r="E54" s="1"/>
-      <c r="H54" s="5" t="s">
-        <v>36</v>
+        <v>15</v>
+      </c>
+      <c r="B54" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="1">
+        <v>42036</v>
+      </c>
+      <c r="F54" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="E55" s="1"/>
       <c r="H55" s="5" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="E56" s="1"/>
       <c r="H56" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="I56" s="7"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="E57" s="1"/>
       <c r="H57" s="5" t="s">
-        <v>39</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="I57" s="7"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" t="s">
-        <v>127</v>
-      </c>
       <c r="E58" s="1"/>
-      <c r="H58" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="H58" s="5"/>
+      <c r="I58" s="7"/>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" t="s">
-        <v>132</v>
+      <c r="B59" t="s">
+        <v>188</v>
+      </c>
+      <c r="D59" t="s">
+        <v>189</v>
       </c>
       <c r="E59" s="1"/>
-      <c r="H59" s="5" t="s">
-        <v>41</v>
+      <c r="F59" t="s">
+        <v>172</v>
+      </c>
+      <c r="G59" t="s">
+        <v>185</v>
+      </c>
+      <c r="H59" s="5"/>
+      <c r="I59" s="7" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" t="s">
-        <v>133</v>
-      </c>
-      <c r="E60" s="1"/>
-      <c r="H60" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="E60" s="2"/>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" t="s">
-        <v>134</v>
-      </c>
-      <c r="E61" s="1"/>
-      <c r="H61" s="5" t="s">
-        <v>43</v>
+      <c r="B61" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" t="s">
+        <v>173</v>
+      </c>
+      <c r="E61" s="1">
+        <v>42036</v>
+      </c>
+      <c r="F61" t="s">
+        <v>8</v>
+      </c>
+      <c r="G61" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E62" s="1"/>
       <c r="H62" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>135</v>
+        <v>125</v>
+      </c>
+      <c r="C63" t="s">
+        <v>179</v>
       </c>
       <c r="E63" s="1"/>
-      <c r="H63" s="5" t="s">
-        <v>45</v>
+      <c r="H63" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E64" s="1"/>
       <c r="H64" s="5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>130</v>
+      </c>
+      <c r="C65" t="s">
+        <v>177</v>
       </c>
       <c r="E65" s="1"/>
-      <c r="H65" s="5" t="s">
-        <v>47</v>
+      <c r="H65" s="10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>137</v>
+        <v>126</v>
+      </c>
+      <c r="C66" t="s">
+        <v>180</v>
       </c>
       <c r="E66" s="1"/>
-      <c r="H66" s="5" t="s">
-        <v>48</v>
+      <c r="H66" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E67" s="1"/>
       <c r="H67" s="5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68" t="s">
+        <v>178</v>
+      </c>
       <c r="E68" s="1"/>
-      <c r="H68" s="5"/>
+      <c r="H68" s="10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>16</v>
-      </c>
-      <c r="B69" t="s">
-        <v>16</v>
-      </c>
-      <c r="E69" s="1">
-        <v>42036</v>
-      </c>
-      <c r="F69" t="s">
-        <v>10</v>
+        <v>133</v>
+      </c>
+      <c r="E69" s="1"/>
+      <c r="H69" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>127</v>
+      </c>
+      <c r="C70" t="s">
+        <v>181</v>
       </c>
       <c r="E70" s="1"/>
-      <c r="H70" s="5" t="s">
-        <v>50</v>
+      <c r="H70" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E71" s="1"/>
       <c r="H71" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I71" s="7"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>140</v>
+        <v>135</v>
+      </c>
+      <c r="C72" t="s">
+        <v>182</v>
       </c>
       <c r="E72" s="1"/>
-      <c r="H72" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I72" s="7"/>
+      <c r="H72" s="10" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>128</v>
+      </c>
+      <c r="C73" t="s">
+        <v>183</v>
+      </c>
       <c r="E73" s="1"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="7"/>
-    </row>
-    <row r="74" spans="1:9" s="4" customFormat="1">
-      <c r="E74" s="6">
+      <c r="H73" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>136</v>
+      </c>
+      <c r="E74" s="1"/>
+      <c r="H74" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" t="s">
+        <v>137</v>
+      </c>
+      <c r="C75" t="s">
+        <v>184</v>
+      </c>
+      <c r="E75" s="1"/>
+      <c r="H75" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="E76" s="1"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="7"/>
+    </row>
+    <row r="77" spans="1:9" s="4" customFormat="1">
+      <c r="D77" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E77" s="6">
         <v>42125</v>
       </c>
-      <c r="F74" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" s="4" customFormat="1">
-      <c r="E75" s="6"/>
-      <c r="H75" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" s="4" customFormat="1">
-      <c r="E76" s="6"/>
-      <c r="H76" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" s="4" customFormat="1">
-      <c r="E77" s="6"/>
-      <c r="H77" s="4" t="s">
-        <v>75</v>
+      <c r="F77" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="4" customFormat="1">
+      <c r="C78" s="4" t="s">
+        <v>187</v>
+      </c>
       <c r="E78" s="6"/>
       <c r="H78" s="4" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="4" customFormat="1">
       <c r="E79" s="6"/>
       <c r="H79" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="81" spans="5:6">
-      <c r="E81" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" s="4" customFormat="1">
+      <c r="E80" s="6"/>
+      <c r="H80" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="81" spans="5:9" s="4" customFormat="1">
+      <c r="E81" s="6"/>
+      <c r="H81" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="82" spans="5:9" s="4" customFormat="1">
+      <c r="E82" s="6"/>
+      <c r="H82" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="84" spans="5:9">
+      <c r="E84" s="1">
         <v>42401</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F84" t="s">
+        <v>175</v>
+      </c>
+      <c r="I84" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="85" spans="5:9">
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="5:9">
+      <c r="E86" s="1">
+        <v>42217</v>
+      </c>
+      <c r="F86" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="5:6">
-      <c r="E82" s="1"/>
-    </row>
-    <row r="83" spans="5:6">
-      <c r="E83" s="1">
-        <v>42217</v>
-      </c>
-      <c r="F83" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D77" r:id="rId1" location="%21Synapse:syn3163039"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
ongoing adventures with covariates tables
</commit_message>
<xml_diff>
--- a/project management/gantt chart.xlsx
+++ b/project management/gantt chart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="197">
   <si>
     <t>TAU data</t>
   </si>
@@ -525,12 +525,6 @@
     <t>I think this is my public root directory. (not sure of working id)</t>
   </si>
   <si>
-    <t>I think this release is the TCX (temporal cotex) samples, n = 399?</t>
-  </si>
-  <si>
-    <t>(I think this should be the CER (cerebellum) samples, n = 374?</t>
-  </si>
-  <si>
     <t>Working Synapse ID - study info</t>
   </si>
   <si>
@@ -589,6 +583,33 @@
   </si>
   <si>
     <t>syn2924460 (or syn2924461 ?)</t>
+  </si>
+  <si>
+    <t>Rush-Broad sample exchange</t>
+  </si>
+  <si>
+    <t>Covariates</t>
+  </si>
+  <si>
+    <t>GeneCounts</t>
+  </si>
+  <si>
+    <t>GeneCounts_Normalized</t>
+  </si>
+  <si>
+    <t>(I think this should be the CER (cerebellum) samples</t>
+  </si>
+  <si>
+    <t>I think this release is the TCX (temporal cotex) samples originating from Mayo Brain Bank and from Banner Sun Health n = 278</t>
+  </si>
+  <si>
+    <t>syn3388564</t>
+  </si>
+  <si>
+    <t>covariates included in the U01_288_AUT_TCx_RNAseq_Covars-Drives_02-06-2015_1447.xlsx spreadheet; data in the mayo-u01-rnaseq s3 bucket (n = 10) synapse ID per Ben L</t>
+  </si>
+  <si>
+    <t>syn2397884</t>
   </si>
 </sst>
 </file>
@@ -674,7 +695,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -730,6 +751,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -752,7 +774,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="56">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -793,6 +815,7 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
@@ -3341,13 +3364,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D59" sqref="D59"/>
+      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3369,7 +3392,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -3406,7 +3429,7 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H4" t="s">
         <v>143</v>
@@ -3956,21 +3979,21 @@
     </row>
     <row r="59" spans="1:9">
       <c r="B59" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D59" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G59" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -3981,7 +4004,7 @@
         <v>16</v>
       </c>
       <c r="D61" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E61" s="1">
         <v>42036</v>
@@ -4007,7 +4030,7 @@
         <v>125</v>
       </c>
       <c r="C63" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E63" s="1"/>
       <c r="H63" s="10" t="s">
@@ -4028,7 +4051,7 @@
         <v>130</v>
       </c>
       <c r="C65" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E65" s="1"/>
       <c r="H65" s="10" t="s">
@@ -4040,7 +4063,7 @@
         <v>126</v>
       </c>
       <c r="C66" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E66" s="1"/>
       <c r="H66" s="10" t="s">
@@ -4061,7 +4084,7 @@
         <v>132</v>
       </c>
       <c r="C68" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E68" s="1"/>
       <c r="H68" s="10" t="s">
@@ -4082,7 +4105,7 @@
         <v>127</v>
       </c>
       <c r="C70" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E70" s="1"/>
       <c r="H70" s="10" t="s">
@@ -4103,7 +4126,7 @@
         <v>135</v>
       </c>
       <c r="C72" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E72" s="1"/>
       <c r="H72" s="10" t="s">
@@ -4115,7 +4138,7 @@
         <v>128</v>
       </c>
       <c r="C73" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E73" s="1"/>
       <c r="H73" s="10" t="s">
@@ -4136,7 +4159,7 @@
         <v>137</v>
       </c>
       <c r="C75" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E75" s="1"/>
       <c r="H75" s="10" t="s">
@@ -4149,22 +4172,25 @@
       <c r="I76" s="7"/>
     </row>
     <row r="77" spans="1:9" s="4" customFormat="1">
+      <c r="C77" s="4" t="s">
+        <v>169</v>
+      </c>
       <c r="D77" s="4" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="E77" s="6">
         <v>42125</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="4" customFormat="1">
       <c r="C78" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E78" s="6"/>
       <c r="H78" s="4" t="s">
@@ -4183,33 +4209,33 @@
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="5:9" s="4" customFormat="1">
+    <row r="81" spans="4:9" s="4" customFormat="1">
       <c r="E81" s="6"/>
       <c r="H81" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="5:9" s="4" customFormat="1">
+    <row r="82" spans="4:9" s="4" customFormat="1">
       <c r="E82" s="6"/>
       <c r="H82" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="5:9">
+    <row r="84" spans="4:9">
       <c r="E84" s="1">
         <v>42401</v>
       </c>
       <c r="F84" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I84" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="85" spans="5:9">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="85" spans="4:9">
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="5:9">
+    <row r="86" spans="4:9">
       <c r="E86" s="1">
         <v>42217</v>
       </c>
@@ -4217,9 +4243,41 @@
         <v>11</v>
       </c>
     </row>
+    <row r="88" spans="4:9" s="4" customFormat="1">
+      <c r="D88" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E88" s="6">
+        <v>42125</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="89" spans="4:9" s="4" customFormat="1">
+      <c r="H89" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="90" spans="4:9" s="4" customFormat="1">
+      <c r="H90" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="91" spans="4:9" s="4" customFormat="1">
+      <c r="H91" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D77" r:id="rId1" location="%21Synapse:syn3163039"/>
+    <hyperlink ref="C77" r:id="rId1" location="%21Synapse:syn3163039"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
chugging on MBB processing, too
</commit_message>
<xml_diff>
--- a/project management/gantt chart.xlsx
+++ b/project management/gantt chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33440" windowHeight="20900" tabRatio="500"/>
+    <workbookView xWindow="980" yWindow="600" windowWidth="33440" windowHeight="26380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="210">
   <si>
     <t>TAU data</t>
   </si>
@@ -543,9 +543,6 @@
     <t>mayo-cer-rna-seq</t>
   </si>
   <si>
-    <t>parent of pilot studies, cer, and tcx samples</t>
-  </si>
-  <si>
     <t>syn3191070</t>
   </si>
   <si>
@@ -585,9 +582,6 @@
     <t>syn2924460 (or syn2924461 ?)</t>
   </si>
   <si>
-    <t>Rush-Broad sample exchange</t>
-  </si>
-  <si>
     <t>Covariates</t>
   </si>
   <si>
@@ -603,20 +597,65 @@
     <t>I think this release is the TCX (temporal cotex) samples originating from Mayo Brain Bank and from Banner Sun Health n = 278</t>
   </si>
   <si>
-    <t>syn3388564</t>
-  </si>
-  <si>
-    <t>covariates included in the U01_288_AUT_TCx_RNAseq_Covars-Drives_02-06-2015_1447.xlsx spreadheet; data in the mayo-u01-rnaseq s3 bucket (n = 10) synapse ID per Ben L</t>
-  </si>
-  <si>
     <t>syn2397884</t>
+  </si>
+  <si>
+    <t>Spring 2015</t>
+  </si>
+  <si>
+    <t>Tau bam files (from snapr)</t>
+  </si>
+  <si>
+    <t>APP bam files (from snapr)</t>
+  </si>
+  <si>
+    <t>Pilot bam files (from snapr)</t>
+  </si>
+  <si>
+    <t>TCX bam files (from snapr)</t>
+  </si>
+  <si>
+    <t>syn3537579</t>
+  </si>
+  <si>
+    <t>Mt. Sinai RNAseq sample swap</t>
+  </si>
+  <si>
+    <t>Rush-Broad sample swap (ROSMAP)</t>
+  </si>
+  <si>
+    <t>data not yet in hand</t>
+  </si>
+  <si>
+    <t>syn3537577</t>
+  </si>
+  <si>
+    <t>parent of APP and TAU studies</t>
+  </si>
+  <si>
+    <t>parent of EGWAS, pilot studies, cer, and tcx samples</t>
+  </si>
+  <si>
+    <t>parent of MAYO LOAD GWAS Genotypes and LOAD TLR4-5 Genotypes</t>
+  </si>
+  <si>
+    <t>syn3157170</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>parent of IL10 and APP/Tau</t>
+  </si>
+  <si>
+    <t>covariates included in the U01_288_AUT_TCx_RNAseq_Covars-Drives_02-06-2015_1447.xlsx spreadheet; data in the mayo-u01-rnaseq s3 bucket (n = 10)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -661,8 +700,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -685,8 +732,13 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -694,8 +746,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="56">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -752,8 +819,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -773,9 +841,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="56"/>
+    <xf numFmtId="17" fontId="6" fillId="5" borderId="1" xfId="56" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="56">
+  <cellStyles count="57">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="56" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -843,13 +914,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -893,13 +964,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -943,13 +1014,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -993,13 +1064,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1043,13 +1114,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1093,13 +1164,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1143,13 +1214,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1193,13 +1264,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1243,13 +1314,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1293,13 +1364,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1343,13 +1414,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1393,13 +1464,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1443,13 +1514,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1493,13 +1564,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1543,13 +1614,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1593,13 +1664,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1643,13 +1714,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1693,13 +1764,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1743,13 +1814,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1793,13 +1864,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1843,13 +1914,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1893,13 +1964,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1943,13 +2014,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1993,13 +2064,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2043,13 +2114,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2093,13 +2164,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2143,13 +2214,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2193,13 +2264,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2243,13 +2314,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2293,13 +2364,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2343,13 +2414,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2393,13 +2464,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2443,13 +2514,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2493,13 +2564,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2543,13 +2614,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2593,13 +2664,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2643,13 +2714,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2693,13 +2764,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2743,13 +2814,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2793,13 +2864,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2843,13 +2914,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2893,13 +2964,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2943,13 +3014,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2993,13 +3064,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3364,13 +3435,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
+      <selection pane="bottomRight" activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3417,867 +3488,954 @@
     </row>
     <row r="4" spans="1:9">
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E4" s="2">
-        <v>42050</v>
+        <v>206</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>207</v>
       </c>
       <c r="G4" t="s">
-        <v>184</v>
-      </c>
-      <c r="H4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="I5" t="s">
-        <v>78</v>
+        <v>183</v>
+      </c>
+      <c r="I4" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>149</v>
-      </c>
-      <c r="C6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H6" t="s">
-        <v>148</v>
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1">
+        <v>42036</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" t="s">
-        <v>100</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="I7" t="s">
-        <v>80</v>
+        <v>140</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="H7" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" t="s">
-        <v>157</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="H8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" t="s">
-        <v>102</v>
-      </c>
-      <c r="H9" t="s">
-        <v>20</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="H9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" t="s">
-        <v>79</v>
-      </c>
+      <c r="E10" s="1"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" t="s">
-        <v>103</v>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="2">
+        <v>42050</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>183</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>143</v>
+      </c>
+      <c r="I11" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" t="s">
-        <v>105</v>
-      </c>
-      <c r="H12" t="s">
-        <v>23</v>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>144</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="I12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" t="s">
+        <v>147</v>
+      </c>
+      <c r="H13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>105</v>
+      </c>
+      <c r="H19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="16" thickBot="1">
+      <c r="A20" t="s">
         <v>87</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C20" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="8" customFormat="1">
-      <c r="D15" s="8" t="s">
+    <row r="21" spans="1:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E21" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="16" thickTop="1"/>
+    <row r="23" spans="1:9" s="8" customFormat="1">
+      <c r="D23" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G23" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H23" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="8" customFormat="1">
-      <c r="C16" s="8" t="s">
+    <row r="24" spans="1:9" s="8" customFormat="1">
+      <c r="C24" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H24" s="8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="4" customFormat="1">
-      <c r="C17" s="4" t="s">
+    <row r="25" spans="1:9" s="4" customFormat="1">
+      <c r="C25" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="4" customFormat="1">
-      <c r="C18" s="4" t="s">
+    <row r="26" spans="1:9" s="4" customFormat="1">
+      <c r="C26" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="4" customFormat="1">
-      <c r="C19" s="4" t="s">
+    <row r="27" spans="1:9" s="4" customFormat="1">
+      <c r="C27" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H27" s="9" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="4" customFormat="1">
-      <c r="C20" s="4" t="s">
+    <row r="28" spans="1:9" s="4" customFormat="1">
+      <c r="C28" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="4" customFormat="1">
-      <c r="C21" s="4" t="s">
+    <row r="29" spans="1:9" s="4" customFormat="1" ht="16" thickBot="1">
+      <c r="C29" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="2">
+    <row r="30" spans="1:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E30" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="16" thickTop="1"/>
+    <row r="32" spans="1:9">
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="2">
         <v>42050</v>
       </c>
-      <c r="F23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" t="s">
-        <v>106</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="H24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="H25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" t="s">
-        <v>107</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="H26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" t="s">
-        <v>107</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="H27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="B29" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="2">
-        <v>42050</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="F32" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="30">
-      <c r="B30" t="s">
+      <c r="I32" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30">
+      <c r="B33" t="s">
         <v>88</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="G30" s="5" t="s">
+      <c r="E33" s="2"/>
+      <c r="G33" s="5" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="H31" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I31" s="7"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="2"/>
-      <c r="H32" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="I32" s="7"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" t="s">
-        <v>110</v>
-      </c>
-      <c r="E33" s="2"/>
-      <c r="H33" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E34" s="2"/>
       <c r="H34" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:9" ht="30">
-      <c r="B35" t="s">
-        <v>93</v>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" t="s">
+        <v>109</v>
       </c>
       <c r="E35" s="2"/>
-      <c r="G35" s="5" t="s">
-        <v>69</v>
+      <c r="H35" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="I35" s="7"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="E36" s="2"/>
       <c r="H36" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I36" s="7"/>
+        <v>67</v>
+      </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="E37" s="2"/>
       <c r="H37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" ht="30">
+      <c r="B38" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="G38" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" t="s">
+        <v>95</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="H39" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="H40" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="I37" s="7"/>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
-        <v>98</v>
-      </c>
-      <c r="C38" t="s">
-        <v>99</v>
-      </c>
-      <c r="E38" s="2"/>
-      <c r="H38" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="I38" s="7"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="E39" s="2"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="7"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="B40" t="s">
-        <v>17</v>
-      </c>
-      <c r="E40" s="2">
-        <v>42050</v>
-      </c>
-      <c r="F40" t="s">
-        <v>7</v>
-      </c>
+      <c r="I40" s="7"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>98</v>
+      </c>
+      <c r="C41" t="s">
+        <v>99</v>
       </c>
       <c r="E41" s="2"/>
       <c r="H41" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" t="s">
-        <v>113</v>
-      </c>
       <c r="E42" s="2"/>
-      <c r="H42" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="H42" s="5"/>
       <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" t="s">
-        <v>114</v>
-      </c>
-      <c r="E43" s="2"/>
-      <c r="H43" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I43" s="7"/>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="2">
+        <v>42050</v>
+      </c>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E44" s="2"/>
       <c r="H44" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I44" s="7"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E45" s="2"/>
       <c r="H45" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E46" s="2"/>
       <c r="H46" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E47" s="2"/>
       <c r="H47" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E48" s="2"/>
       <c r="H48" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I48" s="7"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E49" s="2"/>
       <c r="H49" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I49" s="7"/>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E50" s="2"/>
       <c r="H50" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I50" s="7"/>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E51" s="2"/>
       <c r="H51" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I51" s="7"/>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E52" s="2"/>
       <c r="H52" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I52" s="7"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="E53" s="1"/>
-      <c r="H53" s="5"/>
+      <c r="A53" t="s">
+        <v>121</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="H53" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I53" s="7"/>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B54" t="s">
-        <v>15</v>
-      </c>
-      <c r="E54" s="1">
-        <v>42036</v>
-      </c>
-      <c r="F54" t="s">
-        <v>10</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="H54" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I54" s="7"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>140</v>
-      </c>
-      <c r="E55" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="E55" s="2"/>
       <c r="H55" s="5" t="s">
-        <v>49</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="I55" s="7"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" t="s">
-        <v>138</v>
-      </c>
       <c r="E56" s="1"/>
-      <c r="H56" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I56" s="7"/>
+      <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" t="s">
-        <v>139</v>
+      <c r="B57" t="s">
+        <v>185</v>
+      </c>
+      <c r="D57" t="s">
+        <v>186</v>
       </c>
       <c r="E57" s="1"/>
-      <c r="H57" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I57" s="7"/>
+      <c r="F57" t="s">
+        <v>170</v>
+      </c>
+      <c r="G57" t="s">
+        <v>182</v>
+      </c>
+      <c r="H57" s="5"/>
+      <c r="I57" s="7" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="58" spans="1:9">
-      <c r="E58" s="1"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="7"/>
+      <c r="E58" s="2"/>
     </row>
     <row r="59" spans="1:9">
       <c r="B59" t="s">
-        <v>186</v>
-      </c>
-      <c r="D59" t="s">
-        <v>187</v>
-      </c>
-      <c r="E59" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="E59" s="2">
+        <v>42050</v>
+      </c>
       <c r="F59" t="s">
-        <v>170</v>
-      </c>
-      <c r="G59" t="s">
-        <v>183</v>
-      </c>
-      <c r="H59" s="5"/>
-      <c r="I59" s="7" t="s">
-        <v>174</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" t="s">
+        <v>106</v>
+      </c>
       <c r="E60" s="2"/>
+      <c r="H60" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="61" spans="1:9">
-      <c r="B61" t="s">
-        <v>16</v>
-      </c>
-      <c r="D61" t="s">
-        <v>171</v>
-      </c>
-      <c r="E61" s="1">
-        <v>42036</v>
-      </c>
-      <c r="F61" t="s">
-        <v>8</v>
-      </c>
-      <c r="G61" t="s">
-        <v>9</v>
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" t="s">
+        <v>106</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="H61" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>124</v>
-      </c>
-      <c r="E62" s="1"/>
-      <c r="H62" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="C62" t="s">
+        <v>107</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="H62" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" t="s">
+        <v>107</v>
+      </c>
+      <c r="E63" s="2"/>
+      <c r="H63" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="B65" t="s">
+        <v>16</v>
+      </c>
+      <c r="D65" t="s">
+        <v>171</v>
+      </c>
+      <c r="E65" s="1">
+        <v>42036</v>
+      </c>
+      <c r="F65" t="s">
+        <v>8</v>
+      </c>
+      <c r="G65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" t="s">
+        <v>124</v>
+      </c>
+      <c r="E66" s="1"/>
+      <c r="H66" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
         <v>125</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C67" t="s">
+        <v>176</v>
+      </c>
+      <c r="E67" s="1"/>
+      <c r="H67" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" t="s">
+        <v>129</v>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="H68" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" t="s">
+        <v>130</v>
+      </c>
+      <c r="C69" t="s">
+        <v>174</v>
+      </c>
+      <c r="E69" s="1"/>
+      <c r="H69" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
+        <v>126</v>
+      </c>
+      <c r="C70" t="s">
         <v>177</v>
-      </c>
-      <c r="E63" s="1"/>
-      <c r="H63" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" t="s">
-        <v>129</v>
-      </c>
-      <c r="E64" s="1"/>
-      <c r="H64" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="A65" t="s">
-        <v>130</v>
-      </c>
-      <c r="C65" t="s">
-        <v>175</v>
-      </c>
-      <c r="E65" s="1"/>
-      <c r="H65" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="A66" t="s">
-        <v>126</v>
-      </c>
-      <c r="C66" t="s">
-        <v>178</v>
-      </c>
-      <c r="E66" s="1"/>
-      <c r="H66" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" t="s">
-        <v>131</v>
-      </c>
-      <c r="E67" s="1"/>
-      <c r="H67" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
-      <c r="A68" t="s">
-        <v>132</v>
-      </c>
-      <c r="C68" t="s">
-        <v>176</v>
-      </c>
-      <c r="E68" s="1"/>
-      <c r="H68" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
-      <c r="A69" t="s">
-        <v>133</v>
-      </c>
-      <c r="E69" s="1"/>
-      <c r="H69" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
-      <c r="A70" t="s">
-        <v>127</v>
-      </c>
-      <c r="C70" t="s">
-        <v>179</v>
       </c>
       <c r="E70" s="1"/>
       <c r="H70" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E71" s="1"/>
       <c r="H71" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C72" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E72" s="1"/>
       <c r="H72" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>133</v>
+      </c>
+      <c r="E73" s="1"/>
+      <c r="H73" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>127</v>
+      </c>
+      <c r="C74" t="s">
+        <v>178</v>
+      </c>
+      <c r="E74" s="1"/>
+      <c r="H74" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" t="s">
+        <v>134</v>
+      </c>
+      <c r="E75" s="1"/>
+      <c r="H75" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>135</v>
+      </c>
+      <c r="C76" t="s">
+        <v>179</v>
+      </c>
+      <c r="E76" s="1"/>
+      <c r="H76" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
-      <c r="A73" t="s">
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
         <v>128</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C77" t="s">
+        <v>180</v>
+      </c>
+      <c r="E77" s="1"/>
+      <c r="H77" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" t="s">
+        <v>136</v>
+      </c>
+      <c r="E78" s="1"/>
+      <c r="H78" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="16" thickBot="1">
+      <c r="A79" t="s">
+        <v>137</v>
+      </c>
+      <c r="C79" t="s">
         <v>181</v>
       </c>
-      <c r="E73" s="1"/>
-      <c r="H73" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74" t="s">
-        <v>136</v>
-      </c>
-      <c r="E74" s="1"/>
-      <c r="H74" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
-      <c r="A75" t="s">
-        <v>137</v>
-      </c>
-      <c r="C75" t="s">
-        <v>182</v>
-      </c>
-      <c r="E75" s="1"/>
-      <c r="H75" s="10" t="s">
+      <c r="E79" s="1"/>
+      <c r="H79" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
-      <c r="E76" s="1"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="7"/>
-    </row>
-    <row r="77" spans="1:9" s="4" customFormat="1">
-      <c r="C77" s="4" t="s">
+    <row r="80" spans="1:8" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E80" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="H80" s="11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="81" spans="3:9" ht="16" thickTop="1">
+      <c r="E81" s="1"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="7"/>
+    </row>
+    <row r="82" spans="3:9" s="4" customFormat="1">
+      <c r="C82" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D77" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E77" s="6">
+      <c r="D82" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E82" s="6">
         <v>42125</v>
       </c>
-      <c r="F77" s="4" t="s">
+      <c r="F82" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="I77" s="4" t="s">
+      <c r="I82" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="83" spans="3:9" s="4" customFormat="1">
+      <c r="C83" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E83" s="6"/>
+      <c r="H83" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="3:9" s="4" customFormat="1">
+      <c r="E84" s="6"/>
+      <c r="H84" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="3:9" s="4" customFormat="1">
+      <c r="E85" s="6"/>
+      <c r="H85" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="86" spans="3:9" s="4" customFormat="1">
+      <c r="E86" s="6"/>
+      <c r="H86" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="87" spans="3:9" s="4" customFormat="1" ht="16" thickBot="1">
+      <c r="E87" s="6"/>
+      <c r="H87" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="88" spans="3:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E88" s="11" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" s="4" customFormat="1">
-      <c r="C78" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="E78" s="6"/>
-      <c r="H78" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" s="4" customFormat="1">
-      <c r="E79" s="6"/>
-      <c r="H79" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" s="4" customFormat="1">
-      <c r="E80" s="6"/>
-      <c r="H80" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="81" spans="4:9" s="4" customFormat="1">
-      <c r="E81" s="6"/>
-      <c r="H81" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="82" spans="4:9" s="4" customFormat="1">
-      <c r="E82" s="6"/>
-      <c r="H82" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="84" spans="4:9">
-      <c r="E84" s="1">
+      <c r="H88" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="89" spans="3:9" ht="17" thickTop="1" thickBot="1"/>
+    <row r="90" spans="3:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E90" s="12">
         <v>42401</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F90" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="I84" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="85" spans="4:9">
-      <c r="E85" s="1"/>
-    </row>
-    <row r="86" spans="4:9">
-      <c r="E86" s="1">
+      <c r="I90" s="11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="91" spans="3:9" ht="17" thickTop="1" thickBot="1">
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="3:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E92" s="12">
         <v>42217</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F92" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="4:9" s="4" customFormat="1">
-      <c r="D88" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E88" s="6">
+    <row r="93" spans="3:9" ht="16" thickTop="1"/>
+    <row r="94" spans="3:9" s="4" customFormat="1">
+      <c r="D94" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="E94" s="6">
         <v>42125</v>
       </c>
-      <c r="F88" s="4" t="s">
+      <c r="F94" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I94" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="95" spans="3:9" s="4" customFormat="1">
+      <c r="H95" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="96" spans="3:9" s="4" customFormat="1">
+      <c r="H96" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="G88" s="4" t="s">
+    </row>
+    <row r="97" spans="4:9" s="4" customFormat="1">
+      <c r="H97" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="98" spans="4:9" ht="16" thickBot="1"/>
+    <row r="99" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="D99" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F99" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="G99" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I88" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="89" spans="4:9" s="4" customFormat="1">
-      <c r="H89" s="4" t="s">
+      <c r="I99" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="100" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="H100" s="11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="101" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="H101" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="102" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="H102" s="11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="90" spans="4:9" s="4" customFormat="1">
-      <c r="H90" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="91" spans="4:9" s="4" customFormat="1">
-      <c r="H91" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
+    <row r="103" spans="4:9" ht="16" thickTop="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C77" r:id="rId1" location="%21Synapse:syn3163039"/>
+    <hyperlink ref="C82" r:id="rId1" location="%21Synapse:syn3163039"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
fixing up annotation code
</commit_message>
<xml_diff>
--- a/project management/gantt chart.xlsx
+++ b/project management/gantt chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="600" windowWidth="33440" windowHeight="26380" tabRatio="500"/>
+    <workbookView xWindow="420" yWindow="140" windowWidth="28000" windowHeight="21260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="217">
   <si>
     <t>TAU data</t>
   </si>
@@ -477,18 +477,6 @@
     <t>syn3439202</t>
   </si>
   <si>
-    <t>TAUAPPms_UFL-Mayo_ISB_IlluminaHiSeq2000_App_GeneCounts</t>
-  </si>
-  <si>
-    <t>TAUAPPms_UFL-Mayo_ISB_IlluminaHiSeq2000_App_GeneCounts_Normalized</t>
-  </si>
-  <si>
-    <t>TAUAPPms_UFL-Mayo_ISB_IlluminaHiSeq2000_App_TranscriptCounts</t>
-  </si>
-  <si>
-    <t>TAUAPPms_UFL-Mayo_ISB_IlluminaHiSeq2000_App_TranscriptCounts_Normalized</t>
-  </si>
-  <si>
     <t>syn3483880</t>
   </si>
   <si>
@@ -579,9 +567,6 @@
     <t>syn2910255</t>
   </si>
   <si>
-    <t>syn2924460 (or syn2924461 ?)</t>
-  </si>
-  <si>
     <t>Covariates</t>
   </si>
   <si>
@@ -597,9 +582,6 @@
     <t>I think this release is the TCX (temporal cotex) samples originating from Mayo Brain Bank and from Banner Sun Health n = 278</t>
   </si>
   <si>
-    <t>syn2397884</t>
-  </si>
-  <si>
     <t>Spring 2015</t>
   </si>
   <si>
@@ -649,6 +631,45 @@
   </si>
   <si>
     <t>covariates included in the U01_288_AUT_TCx_RNAseq_Covars-Drives_02-06-2015_1447.xlsx spreadheet; data in the mayo-u01-rnaseq s3 bucket (n = 10)</t>
+  </si>
+  <si>
+    <t>AMP-AD_TAUAPPms_UFL-Mayo_ISB_IlluminaHiSeq2000_App_GeneCounts</t>
+  </si>
+  <si>
+    <t>AMP-AD_TAUAPPms_UFL-Mayo_ISB_IlluminaHiSeq2000_App_GeneCounts_Normalized</t>
+  </si>
+  <si>
+    <t>AMP-AD_TAUAPPms_UFL-Mayo_ISB_IlluminaHiSeq2000_App_TranscriptCounts</t>
+  </si>
+  <si>
+    <t>AMP-AD_TAUAPPms_UFL-Mayo_ISB_IlluminaHiSeq2000_App_TranscriptCounts_Normalized</t>
+  </si>
+  <si>
+    <t>syn2924445</t>
+  </si>
+  <si>
+    <t>syn2924457</t>
+  </si>
+  <si>
+    <t>rnaseq-counts.zip</t>
+  </si>
+  <si>
+    <t>not to migrate</t>
+  </si>
+  <si>
+    <t>double check if needed</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>not to Migrate</t>
+  </si>
+  <si>
+    <t>syn2924460</t>
+  </si>
+  <si>
+    <t>To Get from Steve Younkin (data not in hand)</t>
   </si>
 </sst>
 </file>
@@ -762,7 +783,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -820,6 +841,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -844,7 +877,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="56"/>
     <xf numFmtId="17" fontId="6" fillId="5" borderId="1" xfId="56" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="69">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="56" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -887,6 +920,18 @@
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
@@ -2214,13 +2259,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2264,13 +2309,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3435,13 +3480,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A95" sqref="A95"/>
+      <selection pane="bottomRight" activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3463,7 +3508,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -3474,30 +3519,33 @@
     </row>
     <row r="2" spans="1:9">
       <c r="B2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="B4" t="s">
-        <v>206</v>
+        <v>200</v>
+      </c>
+      <c r="D4" t="s">
+        <v>208</v>
       </c>
       <c r="F4" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3507,11 +3555,17 @@
       <c r="B6" t="s">
         <v>15</v>
       </c>
+      <c r="D6" t="s">
+        <v>209</v>
+      </c>
       <c r="E6" s="1">
         <v>42036</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3562,13 +3616,13 @@
         <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H11" t="s">
         <v>143</v>
       </c>
       <c r="I11" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -3607,7 +3661,7 @@
         <v>100</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I14" t="s">
         <v>80</v>
@@ -3621,7 +3675,7 @@
         <v>101</v>
       </c>
       <c r="H15" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3687,21 +3741,21 @@
     </row>
     <row r="21" spans="1:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="E21" s="11" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="16" thickTop="1"/>
-    <row r="23" spans="1:9" s="8" customFormat="1">
-      <c r="D23" s="8" t="s">
+    <row r="23" spans="1:9" s="4" customFormat="1">
+      <c r="D23" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3712,53 +3766,56 @@
       <c r="H24" s="8" t="s">
         <v>150</v>
       </c>
+      <c r="I24" s="8" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1">
       <c r="C25" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="4" customFormat="1">
       <c r="C26" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>152</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="4" customFormat="1">
       <c r="C27" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>153</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="4" customFormat="1">
       <c r="C28" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>154</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="4" customFormat="1" ht="16" thickBot="1">
       <c r="C29" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>155</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
       <c r="E30" s="11" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="16" thickTop="1"/>
@@ -3773,7 +3830,7 @@
         <v>6</v>
       </c>
       <c r="I32" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30">
@@ -4020,422 +4077,481 @@
       </c>
       <c r="I55" s="7"/>
     </row>
-    <row r="56" spans="1:9">
-      <c r="E56" s="1"/>
+    <row r="56" spans="1:9" ht="16" thickBot="1">
+      <c r="E56" s="2"/>
       <c r="H56" s="5"/>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="B57" t="s">
-        <v>185</v>
-      </c>
-      <c r="D57" t="s">
-        <v>186</v>
-      </c>
-      <c r="E57" s="1"/>
-      <c r="F57" t="s">
-        <v>170</v>
-      </c>
-      <c r="G57" t="s">
-        <v>182</v>
-      </c>
-      <c r="H57" s="5"/>
-      <c r="I57" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="E58" s="2"/>
+      <c r="I56" s="7"/>
+    </row>
+    <row r="57" spans="1:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E57" s="12">
+        <v>42217</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="16" thickTop="1">
+      <c r="E58" s="1"/>
+      <c r="H58" s="5"/>
     </row>
     <row r="59" spans="1:9">
       <c r="B59" t="s">
+        <v>181</v>
+      </c>
+      <c r="D59" t="s">
+        <v>215</v>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="F59" t="s">
+        <v>166</v>
+      </c>
+      <c r="G59" t="s">
+        <v>178</v>
+      </c>
+      <c r="H59" s="5"/>
+      <c r="I59" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="B61" t="s">
         <v>19</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E61" s="2">
         <v>42050</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F61" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" t="s">
-        <v>31</v>
-      </c>
-      <c r="C60" t="s">
-        <v>106</v>
-      </c>
-      <c r="E60" s="2"/>
-      <c r="H60" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" t="s">
-        <v>32</v>
-      </c>
-      <c r="C61" t="s">
-        <v>106</v>
-      </c>
-      <c r="E61" s="2"/>
-      <c r="H61" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C62" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E62" s="2"/>
       <c r="H62" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E63" s="2"/>
       <c r="H63" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" t="s">
+        <v>107</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="H64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" t="s">
+        <v>107</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="H65" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
-      <c r="E64" s="2"/>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="B65" t="s">
+    <row r="66" spans="1:8">
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="B67" t="s">
         <v>16</v>
       </c>
-      <c r="D65" t="s">
-        <v>171</v>
-      </c>
-      <c r="E65" s="1">
+      <c r="D67" t="s">
+        <v>167</v>
+      </c>
+      <c r="E67" s="1">
         <v>42036</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F67" t="s">
         <v>8</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G67" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="A66" t="s">
-        <v>124</v>
-      </c>
-      <c r="E66" s="1"/>
-      <c r="H66" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="A67" t="s">
-        <v>125</v>
-      </c>
-      <c r="C67" t="s">
-        <v>176</v>
-      </c>
-      <c r="E67" s="1"/>
-      <c r="H67" s="10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E68" s="1"/>
       <c r="H68" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C69" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E69" s="1"/>
       <c r="H69" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>126</v>
-      </c>
-      <c r="C70" t="s">
-        <v>177</v>
+        <v>129</v>
       </c>
       <c r="E70" s="1"/>
-      <c r="H70" s="10" t="s">
-        <v>39</v>
+      <c r="H70" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="C71" t="s">
+        <v>170</v>
       </c>
       <c r="E71" s="1"/>
-      <c r="H71" s="5" t="s">
-        <v>40</v>
+      <c r="H71" s="10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C72" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E72" s="1"/>
       <c r="H72" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E73" s="1"/>
       <c r="H73" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C74" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E74" s="1"/>
       <c r="H74" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E75" s="1"/>
       <c r="H75" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C76" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E76" s="1"/>
       <c r="H76" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>128</v>
-      </c>
-      <c r="C77" t="s">
-        <v>180</v>
+        <v>134</v>
       </c>
       <c r="E77" s="1"/>
-      <c r="H77" s="10" t="s">
-        <v>46</v>
+      <c r="H77" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="C78" t="s">
+        <v>175</v>
       </c>
       <c r="E78" s="1"/>
-      <c r="H78" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="16" thickBot="1">
+      <c r="H78" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C79" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E79" s="1"/>
       <c r="H79" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>136</v>
+      </c>
+      <c r="E80" s="1"/>
+      <c r="H80" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="16" thickBot="1">
+      <c r="A81" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81" t="s">
+        <v>177</v>
+      </c>
+      <c r="E81" s="1"/>
+      <c r="H81" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="80" spans="1:8" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="E80" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="H80" s="11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="81" spans="3:9" ht="16" thickTop="1">
-      <c r="E81" s="1"/>
-      <c r="H81" s="5"/>
-      <c r="I81" s="7"/>
-    </row>
-    <row r="82" spans="3:9" s="4" customFormat="1">
-      <c r="C82" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E82" s="6">
+    <row r="82" spans="1:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E82" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="H82" s="11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="16" thickTop="1">
+      <c r="E83" s="1"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="7"/>
+    </row>
+    <row r="84" spans="1:9" s="4" customFormat="1">
+      <c r="C84" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E84" s="6">
         <v>42125</v>
       </c>
-      <c r="F82" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="I82" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="83" spans="3:9" s="4" customFormat="1">
-      <c r="C83" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="E83" s="6"/>
-      <c r="H83" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="3:9" s="4" customFormat="1">
-      <c r="E84" s="6"/>
-      <c r="H84" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="85" spans="3:9" s="4" customFormat="1">
+      <c r="F84" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G84" t="s">
+        <v>9</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="4" customFormat="1">
+      <c r="C85" s="4" t="s">
+        <v>180</v>
+      </c>
       <c r="E85" s="6"/>
       <c r="H85" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="86" spans="3:9" s="4" customFormat="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" s="4" customFormat="1">
       <c r="E86" s="6"/>
       <c r="H86" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="87" spans="3:9" s="4" customFormat="1" ht="16" thickBot="1">
+        <v>210</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="4" customFormat="1">
       <c r="E87" s="6"/>
       <c r="H87" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="4" customFormat="1">
+      <c r="E88" s="6"/>
+      <c r="H88" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" s="4" customFormat="1">
+      <c r="E89" s="6"/>
+      <c r="H89" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" s="4" customFormat="1" ht="16" thickBot="1">
+      <c r="E90" s="6"/>
+      <c r="H90" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="88" spans="3:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="E88" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="H88" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="89" spans="3:9" ht="17" thickTop="1" thickBot="1"/>
-    <row r="90" spans="3:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="E90" s="12">
+    <row r="91" spans="1:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E91" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="H91" s="11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="17" thickTop="1" thickBot="1"/>
+    <row r="93" spans="1:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="E93" s="12">
         <v>42401</v>
       </c>
-      <c r="F90" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="I90" s="11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="91" spans="3:9" ht="17" thickTop="1" thickBot="1">
-      <c r="E91" s="1"/>
-    </row>
-    <row r="92" spans="3:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="E92" s="12">
-        <v>42217</v>
-      </c>
-      <c r="F92" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="93" spans="3:9" ht="16" thickTop="1"/>
-    <row r="94" spans="3:9" s="4" customFormat="1">
-      <c r="D94" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="E94" s="6">
+      <c r="F93" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="I93" s="11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="16" thickTop="1">
+      <c r="E94" s="1"/>
+    </row>
+    <row r="95" spans="1:9" s="4" customFormat="1">
+      <c r="D95" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E95" s="6">
         <v>42125</v>
       </c>
-      <c r="F94" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="G94" s="4" t="s">
+      <c r="F95" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="G95" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I94" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="95" spans="3:9" s="4" customFormat="1">
-      <c r="H95" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="96" spans="3:9" s="4" customFormat="1">
+      <c r="I95" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" s="4" customFormat="1">
       <c r="H96" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="97" spans="4:9" s="4" customFormat="1">
       <c r="H97" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="98" spans="4:9" ht="16" thickBot="1"/>
-    <row r="99" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="D99" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="F99" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="G99" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="I97" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="98" spans="4:9" s="4" customFormat="1">
+      <c r="H98" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="99" spans="4:9" s="4" customFormat="1">
+      <c r="H99" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100" spans="4:9" s="4" customFormat="1">
+      <c r="H100" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I100" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="101" spans="4:9" s="4" customFormat="1">
+      <c r="H101" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I101" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="102" spans="4:9" ht="16" thickBot="1"/>
+    <row r="103" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="D103" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="E103" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="F103" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="G103" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I99" s="11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="100" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="H100" s="11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="101" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="H101" s="11" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="102" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
-      <c r="H102" s="11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="103" spans="4:9" ht="16" thickTop="1"/>
+      <c r="I103" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="104" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="H104" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="105" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="H105" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="106" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="H106" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="107" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="H107" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I107" s="11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="108" spans="4:9" s="11" customFormat="1" ht="17" thickTop="1" thickBot="1">
+      <c r="H108" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I108" s="11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="109" spans="4:9" ht="16" thickTop="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C82" r:id="rId1" location="%21Synapse:syn3163039"/>
+    <hyperlink ref="C84" r:id="rId1" location="%21Synapse:syn3163039"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>